<commit_message>
changes to BOM as requested by Armin Brandl
</commit_message>
<xml_diff>
--- a/eagle/BOMs/BOMs_WatchPLB.xlsx
+++ b/eagle/BOMs/BOMs_WatchPLB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Git\eagle\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E271DFB-FB42-4BDA-AC62-F520C774EC45}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C74DE9-5DB0-403D-9CA5-76C4CA456101}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">GPS_Board!$A$1:$F$7</definedName>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Mainboard!$A$1:$H$92</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Mainboard!$A$1:$H$94</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="368">
   <si>
     <t>Qty</t>
   </si>
@@ -209,9 +209,6 @@
     <t>C38, C39, C40, C41, C44, C45, C46, C47, C49</t>
   </si>
   <si>
-    <t xml:space="preserve">100uF  647-GYA1E101MCQ1GS </t>
-  </si>
-  <si>
     <t>CPOL-EUE</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>C9</t>
   </si>
   <si>
-    <t xml:space="preserve">10uF  80-EDK106M025A9DAA  </t>
-  </si>
-  <si>
     <t>C53, C56, C59</t>
   </si>
   <si>
@@ -269,9 +263,6 @@
     <t>R52</t>
   </si>
   <si>
-    <t>16MHz_LFXTAL051370Reel</t>
-  </si>
-  <si>
     <t>CRYSTALHC49UP</t>
   </si>
   <si>
@@ -281,9 +272,6 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>CRYSTAL</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
@@ -323,9 +311,6 @@
     <t>R9, R23, R24</t>
   </si>
   <si>
-    <t xml:space="preserve">22uF 80-EDK226M050A9GAA </t>
-  </si>
-  <si>
     <t>C48, C51, C52</t>
   </si>
   <si>
@@ -371,9 +356,6 @@
     <t>R41</t>
   </si>
   <si>
-    <t xml:space="preserve">4.7uF low esr 80-T521B475M35ATE150 </t>
-  </si>
-  <si>
     <t>CPOL-EUB/3528-21R</t>
   </si>
   <si>
@@ -431,9 +413,6 @@
     <t>C28, C31</t>
   </si>
   <si>
-    <t xml:space="preserve">8MHz / LFXTAL020423Reel </t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -1113,13 +1092,64 @@
   </si>
   <si>
     <t>https://www.mouser.at/ProductDetail/Bridgetek/VA-FC-1M-BKW?qs=sGAEpiMZZMsvnOgGvSjZeNycs%252bzgSdByftKjNyBvcRw%3d</t>
+  </si>
+  <si>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLARIZED CAPACITOR, European symbol,  80-EDK226M050A9GAA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10uF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLARIZED CAPACITOR, European symbol,  80-EDK106M025A9DAA  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">100uF  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLARIZED CAPACITOR, European symbol, 647-GYA1E101MCQ1GS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7uF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLARIZED CAPACITOR, European symbol, low esr 80-T521B475M35ATE150 </t>
+  </si>
+  <si>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>CRYSTAL, 16MHz_LFXTAL051370Reel</t>
+  </si>
+  <si>
+    <t>16MHz_Crystal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRYSTAL, 8MHz / LFXTAL020423Reel </t>
+  </si>
+  <si>
+    <t>8MHz-Crystal</t>
+  </si>
+  <si>
+    <t>Pinheader Male 2.54mm</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/10Pcs-Lot-40-Pin-2-54mm-1x40-pin-Heigth-11-34MM-Single-Row-Male-straight-male/32873942371.html</t>
+  </si>
+  <si>
+    <t>Pinheader Female 2.54mm</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/10Pcs-Lot-40Pin-2-54mm-1x40-pin-socket-Single-Row-Female-straight-female-Pin-Header-Connector/32892752726.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1250,6 +1280,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1552,7 +1590,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1595,12 +1633,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1634,6 +1675,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1757,8 +1799,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="BOM_watchplb_mainboard_v1_03" displayName="BOM_watchplb_mainboard_v1_03" ref="A1:H92" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H92" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="BOM_watchplb_mainboard_v1_03" displayName="BOM_watchplb_mainboard_v1_03" ref="A1:H94" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H94" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState ref="A2:H92">
+    <sortCondition ref="E1:E92"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Qty" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="12"/>
@@ -2086,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H92" sqref="H92"/>
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,6 +2145,7 @@
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="177.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2125,76 +2171,76 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>211</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>213</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>214</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>254</v>
+      <c r="H3" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
@@ -2203,59 +2249,59 @@
         <v>7</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>271</v>
+      <c r="H5" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>272</v>
+      <c r="H6" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2263,51 +2309,51 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>168</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>171</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>273</v>
+      <c r="H7" s="2" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>274</v>
+      <c r="H8" s="2" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2315,51 +2361,51 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>275</v>
+      <c r="H9" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H10" t="s">
-        <v>299</v>
+      <c r="H10" s="2" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2367,33 +2413,33 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>47</v>
+        <v>121</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>276</v>
+      <c r="H11" s="2" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>49</v>
@@ -2402,7 +2448,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>52</v>
@@ -2410,25 +2456,25 @@
       <c r="G12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>300</v>
+      <c r="H12" s="2" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>205</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>206</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>52</v>
@@ -2437,110 +2483,110 @@
         <v>7</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>300</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>301</v>
+      <c r="H14" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>277</v>
+      <c r="H15" s="2" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>296</v>
+        <v>83</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>278</v>
+      <c r="H16" s="2" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>351</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>352</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2549,77 +2595,77 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>353</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>354</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>303</v>
+      <c r="H18" s="2" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>355</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>356</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>279</v>
+      <c r="H19" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>207</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>73</v>
+        <v>208</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>304</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2627,25 +2673,25 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>357</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>31</v>
+        <v>358</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>280</v>
+      <c r="H21" s="2" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2653,25 +2699,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>305</v>
+      <c r="H22" s="2" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2679,285 +2725,285 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>226</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>227</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>39</v>
+        <v>196</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>82</v>
+        <v>228</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H23" t="s">
-        <v>282</v>
+      <c r="H23" s="2" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>39</v>
+        <v>196</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>31</v>
+        <v>198</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>281</v>
+      <c r="H24" s="2" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>359</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>306</v>
+      <c r="H25" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>245</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>87</v>
+        <v>246</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>306</v>
+      <c r="H26" s="2" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>307</v>
+      <c r="H27" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>141</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>144</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>308</v>
+      <c r="H28" s="2" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>93</v>
+        <v>18</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>95</v>
+        <v>193</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>309</v>
+      <c r="H30" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>33</v>
+        <v>150</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>36</v>
+        <v>153</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>310</v>
+      <c r="H31" s="2" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
+        <v>184</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>50</v>
+        <v>185</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>311</v>
+      <c r="H32" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>311</v>
+      <c r="H33" s="2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2965,25 +3011,25 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>39</v>
+        <v>185</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>284</v>
+      <c r="H34" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2991,51 +3037,51 @@
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>104</v>
+        <v>189</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>38</v>
+        <v>184</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>39</v>
+        <v>185</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>105</v>
+        <v>190</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>285</v>
+      <c r="H35" s="2" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>312</v>
+      <c r="H36" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3043,25 +3089,25 @@
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>31</v>
+        <v>157</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>286</v>
+      <c r="H37" s="2" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3069,181 +3115,181 @@
         <v>1</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>239</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>219</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>112</v>
+        <v>220</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>113</v>
+        <v>240</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>313</v>
+      <c r="H38" s="2" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>114</v>
+        <v>218</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>38</v>
+        <v>219</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>115</v>
+        <v>221</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>287</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>288</v>
+      <c r="H40" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>289</v>
+      <c r="H41" s="2" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>290</v>
+      <c r="H42" s="2" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>32</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>123</v>
+        <v>35</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>314</v>
+      <c r="H43" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>39</v>
+        <v>173</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>125</v>
+        <v>174</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>315</v>
+      <c r="H44" s="2" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3251,77 +3297,77 @@
         <v>2</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="2" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>129</v>
+        <v>244</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>317</v>
+      <c r="H46" s="2" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>131</v>
+        <v>182</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>318</v>
+      <c r="H47" s="2" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3329,51 +3375,51 @@
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>132</v>
+        <v>241</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>39</v>
+        <v>147</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>133</v>
+        <v>242</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>291</v>
+      <c r="H48" s="2" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>134</v>
+        <v>224</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>136</v>
+        <v>225</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>319</v>
+      <c r="H49" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3381,77 +3427,77 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>138</v>
+        <v>12</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>140</v>
+        <v>234</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>320</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>142</v>
+        <v>363</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>143</v>
+        <v>74</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>146</v>
+        <v>362</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>321</v>
+      <c r="H51" s="2" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>322</v>
+      <c r="H52" s="2" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3459,25 +3505,25 @@
         <v>2</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>323</v>
+      <c r="H53" s="2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3485,77 +3531,77 @@
         <v>1</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>157</v>
+        <v>361</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>157</v>
+        <v>74</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>158</v>
+        <v>75</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>160</v>
+        <v>360</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>324</v>
+      <c r="H54" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>351</v>
+      <c r="H55" s="2" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>165</v>
+        <v>108</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>166</v>
+        <v>38</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>169</v>
+        <v>31</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>349</v>
+        <v>7</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3563,25 +3609,25 @@
         <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>171</v>
+        <v>46</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>171</v>
+        <v>38</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>172</v>
+        <v>39</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>173</v>
+        <v>47</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>174</v>
+        <v>31</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="1" t="s">
-        <v>325</v>
+      <c r="H57" s="2" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3589,25 +3635,25 @@
         <v>1</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>175</v>
+        <v>287</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>176</v>
+        <v>38</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>178</v>
+        <v>285</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H58" s="1" t="s">
-        <v>326</v>
+      <c r="H58" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3615,51 +3661,49 @@
         <v>1</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>179</v>
+        <v>288</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>179</v>
+        <v>38</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>181</v>
+        <v>286</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>327</v>
+        <v>31</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>114</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>184</v>
+        <v>38</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>185</v>
+        <v>39</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>186</v>
+        <v>115</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>187</v>
+        <v>31</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>328</v>
+      <c r="H60" s="2" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3667,25 +3711,25 @@
         <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>188</v>
+        <v>79</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>153</v>
+        <v>38</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>189</v>
+        <v>80</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>156</v>
+        <v>31</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H61" s="1" t="s">
-        <v>329</v>
+      <c r="H61" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3693,51 +3737,51 @@
         <v>1</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>191</v>
+        <v>28</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>192</v>
+        <v>29</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>193</v>
+        <v>87</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>336</v>
+      <c r="H62" s="2" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>194</v>
+        <v>37</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>191</v>
+        <v>38</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>195</v>
+        <v>40</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H63" s="1" t="s">
-        <v>336</v>
+      <c r="H63" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3745,77 +3789,77 @@
         <v>1</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>196</v>
+        <v>60</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>191</v>
+        <v>38</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>192</v>
+        <v>39</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>197</v>
+        <v>61</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>336</v>
+      <c r="H64" s="2" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>198</v>
+        <v>112</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>198</v>
+        <v>38</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>199</v>
+        <v>39</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>200</v>
+        <v>113</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>201</v>
+        <v>31</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="1" t="s">
-        <v>337</v>
+      <c r="H65" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>202</v>
+        <v>118</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>202</v>
+        <v>38</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>203</v>
+        <v>39</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>204</v>
+        <v>119</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>205</v>
+        <v>31</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>338</v>
+      <c r="H66" s="2" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3823,25 +3867,25 @@
         <v>1</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>206</v>
+        <v>103</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>206</v>
+        <v>38</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>207</v>
+        <v>39</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>208</v>
+        <v>104</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>339</v>
+      <c r="H67" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -3849,77 +3893,77 @@
         <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>209</v>
+        <v>77</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>209</v>
+        <v>38</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>210</v>
+        <v>39</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>211</v>
+        <v>78</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="1" t="s">
-        <v>340</v>
+      <c r="H68" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>212</v>
+        <v>110</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>213</v>
+        <v>111</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H69" s="1" t="s">
-        <v>254</v>
+      <c r="H69" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>214</v>
+        <v>97</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>215</v>
+        <v>98</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="1" t="s">
-        <v>254</v>
+      <c r="H70" s="2" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -3927,7 +3971,7 @@
         <v>1</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>216</v>
+        <v>125</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>38</v>
@@ -3936,7 +3980,7 @@
         <v>39</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>217</v>
+        <v>126</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>31</v>
@@ -3944,60 +3988,60 @@
       <c r="G71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H71" s="1" t="s">
-        <v>343</v>
+      <c r="H71" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>218</v>
+        <v>99</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>218</v>
+        <v>38</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>219</v>
+        <v>39</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H72" s="1" t="s">
-        <v>254</v>
+      <c r="H72" s="2" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>222</v>
+        <v>62</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>222</v>
+        <v>38</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>223</v>
+        <v>39</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>254</v>
+      <c r="H73" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4005,25 +4049,25 @@
         <v>1</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>225</v>
+        <v>27</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>226</v>
+        <v>28</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>227</v>
+        <v>29</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>228</v>
+        <v>30</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="1" t="s">
-        <v>254</v>
+      <c r="H74" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4031,51 +4075,51 @@
         <v>1</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>229</v>
+        <v>68</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>229</v>
+        <v>38</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>229</v>
+        <v>39</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>230</v>
+        <v>69</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H75" s="1" t="s">
-        <v>344</v>
+      <c r="H75" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>231</v>
+        <v>72</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>153</v>
+        <v>38</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>232</v>
+        <v>73</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>156</v>
+        <v>31</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H76" s="1" t="s">
-        <v>330</v>
+      <c r="H76" s="2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4083,51 +4127,51 @@
         <v>1</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>234</v>
+        <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>203</v>
+        <v>39</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>345</v>
+      <c r="H77" s="2" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>236</v>
+        <v>88</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>237</v>
+        <v>38</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>238</v>
+        <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>239</v>
+        <v>89</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H78" s="1" t="s">
-        <v>346</v>
+      <c r="H78" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4135,51 +4179,51 @@
         <v>1</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>12</v>
+        <v>215</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>13</v>
+        <v>216</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>15</v>
+        <v>214</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>242</v>
+        <v>7</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>242</v>
+        <v>19</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>243</v>
+        <v>20</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>244</v>
+        <v>21</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H80" s="1" t="s">
-        <v>347</v>
+      <c r="H80" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4187,25 +4231,25 @@
         <v>1</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H81" s="1" t="s">
-        <v>348</v>
+      <c r="H81" s="2" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4213,25 +4257,25 @@
         <v>1</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>153</v>
+        <v>199</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H82" s="1" t="s">
-        <v>331</v>
+      <c r="H82" s="2" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4239,25 +4283,25 @@
         <v>1</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>153</v>
+        <v>230</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H83" s="1" t="s">
-        <v>335</v>
+      <c r="H83" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4265,25 +4309,25 @@
         <v>1</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>42</v>
+        <v>202</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>43</v>
+        <v>203</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>253</v>
+        <v>204</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="1" t="s">
-        <v>342</v>
+      <c r="H84" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4291,25 +4335,25 @@
         <v>1</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>294</v>
+        <v>235</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>38</v>
+        <v>235</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>39</v>
+        <v>236</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>292</v>
+        <v>237</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>31</v>
+        <v>238</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H85" s="1" t="s">
-        <v>297</v>
+      <c r="H85" s="2" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4317,23 +4361,25 @@
         <v>1</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>295</v>
+        <v>158</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>293</v>
+        <v>161</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1" t="s">
-        <v>298</v>
+        <v>162</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4350,15 +4396,15 @@
         <v>1</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
-      <c r="H88" s="1" t="s">
-        <v>350</v>
+      <c r="H88" s="2" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4366,15 +4412,15 @@
         <v>4</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
-      <c r="H89" s="1" t="s">
-        <v>354</v>
+      <c r="H89" s="2" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4382,15 +4428,15 @@
         <v>1</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="H90" s="1" t="s">
-        <v>352</v>
+      <c r="H90" s="2" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4398,17 +4444,17 @@
         <v>1</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-      <c r="H91" s="1" t="s">
-        <v>355</v>
+      <c r="H91" s="2" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4416,21 +4462,140 @@
         <v>3</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" t="s">
-        <v>357</v>
+      <c r="H92" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{AF0345A8-B47C-4869-919B-269F6D651AE3}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{C731202E-8C42-4533-9430-D0D210D2F04D}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{F4B8B8C2-7B71-442E-BD30-E2ECDE52B83C}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{D14FB558-0400-4498-92C4-56B46D21BC22}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{5DD362B4-5F1C-4FDC-A987-A82743A44EA8}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{9CEAE529-3EC7-4F41-93A5-282F18841EDE}"/>
+    <hyperlink ref="H10" r:id="rId7" xr:uid="{F48F8CFD-B0D9-4AFE-B152-21E16506E0A7}"/>
+    <hyperlink ref="H11" r:id="rId8" xr:uid="{353243A0-006C-46E4-BD7C-B30694C373BD}"/>
+    <hyperlink ref="H12" r:id="rId9" xr:uid="{270A1B97-0628-47B6-8247-FCF5ED57D4EA}"/>
+    <hyperlink ref="H14" r:id="rId10" xr:uid="{430DC2A1-1AF3-464C-85EA-205ABD0234E1}"/>
+    <hyperlink ref="H15" r:id="rId11" xr:uid="{EA9CF757-3C5D-4A9E-9722-C1324684617C}"/>
+    <hyperlink ref="H16" r:id="rId12" xr:uid="{EC1FED56-AE0A-4603-B111-652B5FEC2199}"/>
+    <hyperlink ref="H17" r:id="rId13" xr:uid="{52F16938-ABED-435B-9CCA-6138A9D618D9}"/>
+    <hyperlink ref="H18" r:id="rId14" xr:uid="{47E845A0-F387-40D7-96A9-B9478EE14C94}"/>
+    <hyperlink ref="H19" r:id="rId15" xr:uid="{B20D9231-75FB-4C43-8059-163789FF26F6}"/>
+    <hyperlink ref="H21" r:id="rId16" xr:uid="{E13EAB3E-E0AC-4D49-89D9-0CF73C396A00}"/>
+    <hyperlink ref="H22" r:id="rId17" xr:uid="{2D3FE28D-C210-47AC-BC64-10C0F6F2BB42}"/>
+    <hyperlink ref="H23" r:id="rId18" xr:uid="{1C970058-6948-43F5-A099-2DB6A8AC01D4}"/>
+    <hyperlink ref="H24" r:id="rId19" xr:uid="{7C2AFDF6-564A-4EA2-906A-CCE9089BEA72}"/>
+    <hyperlink ref="H25" r:id="rId20" xr:uid="{2AEFDF37-2563-4BCA-9D9E-1445C812818E}"/>
+    <hyperlink ref="H27" r:id="rId21" xr:uid="{0C3AB61F-F931-4786-8A8A-1EB693DA3CFF}"/>
+    <hyperlink ref="H26" r:id="rId22" xr:uid="{1477C2DA-3FE5-4660-82D8-518113563D93}"/>
+    <hyperlink ref="H28" r:id="rId23" xr:uid="{C4B1E981-34A6-4EF7-B00C-15C58A7B4987}"/>
+    <hyperlink ref="H30" r:id="rId24" xr:uid="{ADCDF6A2-5C29-4188-A1C0-5F3CF20DB6FC}"/>
+    <hyperlink ref="H31" r:id="rId25" xr:uid="{E81595DD-8816-47A0-964D-2312E5F45F52}"/>
+    <hyperlink ref="H32" r:id="rId26" xr:uid="{9EB4D674-C238-432D-9ED4-8F0F1FE664D3}"/>
+    <hyperlink ref="H33" r:id="rId27" xr:uid="{FCB9527C-3E20-4150-8E3C-3FC277FC6717}"/>
+    <hyperlink ref="H34" r:id="rId28" xr:uid="{A312DCD4-F05C-4094-B9DD-B252B256BE76}"/>
+    <hyperlink ref="H35" r:id="rId29" xr:uid="{638C1B80-FD8C-4F30-BB95-86A2ED7D0422}"/>
+    <hyperlink ref="H36" r:id="rId30" xr:uid="{ED7FA15F-C5D1-4CE6-A2A5-F0C3249285DF}"/>
+    <hyperlink ref="H37" r:id="rId31" xr:uid="{2402B262-DED5-47FE-A686-F1BA8C2B2BB5}"/>
+    <hyperlink ref="H38" r:id="rId32" xr:uid="{586913CF-9E67-4EA9-86A5-94F9D2FC0DAA}"/>
+    <hyperlink ref="H40" r:id="rId33" xr:uid="{99FF5EC5-2D07-4E0C-91DC-4E5C10D67088}"/>
+    <hyperlink ref="H41" r:id="rId34" xr:uid="{63C0D3D9-7DDC-4EFE-97FD-A4807C0E6F6A}"/>
+    <hyperlink ref="H42" r:id="rId35" xr:uid="{3E9B107F-4128-40A2-A7DB-B6F6514EC076}"/>
+    <hyperlink ref="H43" r:id="rId36" xr:uid="{70FDA59E-BB39-4814-B256-4989EFD4D65B}"/>
+    <hyperlink ref="H44" r:id="rId37" xr:uid="{FD84E09B-1954-4181-8210-C7289913CA4B}"/>
+    <hyperlink ref="H45" r:id="rId38" xr:uid="{05BE3011-B7B8-461D-91DF-33A95EF67B21}"/>
+    <hyperlink ref="H46" r:id="rId39" xr:uid="{DF528EB6-EFE2-4D96-9170-41120432D00E}"/>
+    <hyperlink ref="H47" r:id="rId40" xr:uid="{6F870EFA-D99F-45E0-B630-693950A75E6A}"/>
+    <hyperlink ref="H48" r:id="rId41" xr:uid="{6B1A1121-0B1A-494D-BCF6-F1D8BB0BCD67}"/>
+    <hyperlink ref="H49" r:id="rId42" xr:uid="{95021D73-ED2D-46D7-8F5A-709B32274CD9}"/>
+    <hyperlink ref="H51" r:id="rId43" xr:uid="{EDC256D1-54B7-4C44-A294-829D6F1BFFC7}"/>
+    <hyperlink ref="H52" r:id="rId44" xr:uid="{D041C63D-6CF1-4142-B15A-330A8A6F3CDE}"/>
+    <hyperlink ref="H53" r:id="rId45" xr:uid="{33A140F6-DAFD-4D25-A9AE-D75B92F43B28}"/>
+    <hyperlink ref="H54" r:id="rId46" xr:uid="{EA5799EB-19FC-4564-A18B-D282479B64CB}"/>
+    <hyperlink ref="H55" r:id="rId47" xr:uid="{9EA1E006-7DA7-4472-955F-0F5C33D3EB6B}"/>
+    <hyperlink ref="H56" r:id="rId48" xr:uid="{22B28C6E-B7E8-41F8-95DD-1C286685B240}"/>
+    <hyperlink ref="H57" r:id="rId49" xr:uid="{69928788-C38D-4E2F-BBE3-3D75CD1C7F26}"/>
+    <hyperlink ref="H58" r:id="rId50" xr:uid="{D3636742-8C49-4ACB-BB67-52FE9655B217}"/>
+    <hyperlink ref="H59" r:id="rId51" xr:uid="{97111B7B-DD10-4B99-86B9-0BE4EDBFCD8F}"/>
+    <hyperlink ref="H60" r:id="rId52" xr:uid="{20159129-A44B-4E97-BA02-AD1FBFEA4B69}"/>
+    <hyperlink ref="H61" r:id="rId53" xr:uid="{3CED28F1-AABF-416E-B7C0-ECC43DCDAC62}"/>
+    <hyperlink ref="H62" r:id="rId54" xr:uid="{C81370BE-0069-4261-BE3D-BF8B150DEE89}"/>
+    <hyperlink ref="H63" r:id="rId55" xr:uid="{E0B7343B-5026-490A-9204-466DBBB9ADAE}"/>
+    <hyperlink ref="H64" r:id="rId56" xr:uid="{05D5C180-3052-47BC-AABA-0DD8BFCB4873}"/>
+    <hyperlink ref="H65" r:id="rId57" xr:uid="{ECD229B1-03EB-40FB-BBA9-E666914BCCAB}"/>
+    <hyperlink ref="H66" r:id="rId58" xr:uid="{AD71A0A8-3115-4953-A87D-C5D48968888C}"/>
+    <hyperlink ref="H67" r:id="rId59" xr:uid="{622363FB-A60E-446E-8FCE-8DDCE19A404F}"/>
+    <hyperlink ref="H68" r:id="rId60" xr:uid="{6DA95BE5-4C22-4731-AC62-C03F378988C7}"/>
+    <hyperlink ref="H69" r:id="rId61" xr:uid="{9B309B5B-516E-4DA9-B4B8-FF1CD77D3844}"/>
+    <hyperlink ref="H70" r:id="rId62" xr:uid="{AA20CDF6-47E2-4EF2-9EE2-0201B5D172ED}"/>
+    <hyperlink ref="H71" r:id="rId63" xr:uid="{73D88107-2063-4D16-836A-D7DD35FA8BA8}"/>
+    <hyperlink ref="H72" r:id="rId64" xr:uid="{9E318F0C-E499-4B2B-85ED-3963EE54841E}"/>
+    <hyperlink ref="H73" r:id="rId65" xr:uid="{909861B1-D635-41F1-BD4E-40B058473D5A}"/>
+    <hyperlink ref="H74" r:id="rId66" xr:uid="{465EFED6-9A1B-4BD9-952F-75D09E5D25EE}"/>
+    <hyperlink ref="H75" r:id="rId67" xr:uid="{416C2F72-C77B-4EE8-B622-F8E724523A30}"/>
+    <hyperlink ref="H76" r:id="rId68" xr:uid="{85DE1729-6FAF-4820-AE38-320843B10186}"/>
+    <hyperlink ref="H77" r:id="rId69" xr:uid="{7C46EF45-5CD2-4A6E-945D-DE761A89A429}"/>
+    <hyperlink ref="H78" r:id="rId70" xr:uid="{02BBC9EC-E9DD-41C4-BC24-B2986AD5B9ED}"/>
+    <hyperlink ref="H80" r:id="rId71" xr:uid="{51FD0953-0962-44B3-86A6-C0E840701570}"/>
+    <hyperlink ref="H81" r:id="rId72" xr:uid="{A7F0B3B6-A3DA-454D-9748-93D7C4294B16}"/>
+    <hyperlink ref="H82" r:id="rId73" xr:uid="{2E3D0B77-7944-4A58-BD92-7FDEFC567861}"/>
+    <hyperlink ref="H83" r:id="rId74" xr:uid="{23261957-D858-4C70-BE6B-45CF4C6D6A04}"/>
+    <hyperlink ref="H84" r:id="rId75" xr:uid="{5F90D62B-78D4-4DC4-B38B-033AFCA1A8A9}"/>
+    <hyperlink ref="H85" r:id="rId76" xr:uid="{A504FDA2-C5C6-437E-835B-C43549C397A5}"/>
+    <hyperlink ref="H86" r:id="rId77" xr:uid="{E30E8BEE-4700-4B4A-ADB5-2B9D5B123727}"/>
+    <hyperlink ref="H88" r:id="rId78" xr:uid="{B4C04F62-26E8-4A7F-8AF1-4502D45146C8}"/>
+    <hyperlink ref="H89" r:id="rId79" xr:uid="{981D863F-2D25-43CE-92B9-6104289E0E6C}"/>
+    <hyperlink ref="H90" r:id="rId80" xr:uid="{382606B6-F67A-47CA-B140-40CE51AA82AC}"/>
+    <hyperlink ref="H91" r:id="rId81" xr:uid="{A9695FEE-1C75-4F90-B13E-9F4D6A52FD46}"/>
+    <hyperlink ref="H92" r:id="rId82" xr:uid="{BCFCA6A7-8CB0-4BF2-B401-615C1F791D76}"/>
+    <hyperlink ref="H93" r:id="rId83" xr:uid="{8E2F0C3D-26F9-46EE-87C0-128291A42BE6}"/>
+    <hyperlink ref="H94" r:id="rId84" xr:uid="{49DAD614-9220-4A57-B6FD-961940DBADD0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId85"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId86"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4472,7 +4637,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4489,7 +4654,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>15</v>
@@ -4501,7 +4666,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
@@ -4510,13 +4675,13 @@
         <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4524,7 +4689,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>49</v>
@@ -4533,13 +4698,13 @@
         <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4547,7 +4712,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>38</v>
@@ -4556,13 +4721,13 @@
         <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -4570,22 +4735,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4593,22 +4758,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Marked received Parts on BOM
</commit_message>
<xml_diff>
--- a/eagle/BOMs/BOMs_WatchPLB.xlsx
+++ b/eagle/BOMs/BOMs_WatchPLB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Git\eagle\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CD94B9-9857-46AC-89A4-70EC18B386F1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A785E58E-CD06-4886-A5A4-948AC2C51D53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">GPS_Board!$A$1:$F$7</definedName>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Mainboard!$A$1:$H$94</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Mainboard!$A$1:$I$94</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="374">
   <si>
     <t>Qty</t>
   </si>
@@ -1149,6 +1149,18 @@
   </si>
   <si>
     <t>DIODE, MMSZ5246BS-7-F</t>
+  </si>
+  <si>
+    <t>Vorhanden</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>3 von 9</t>
   </si>
 </sst>
 </file>
@@ -1641,11 +1653,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" xfId="38" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1692,7 +1706,40 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1747,8 +1794,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="29">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="30">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Qty" tableColumnId="1"/>
       <queryTableField id="2" name="Value" tableColumnId="2"/>
       <queryTableField id="3" name="Device" tableColumnId="3"/>
@@ -1756,6 +1803,7 @@
       <queryTableField id="5" name="Parts" tableColumnId="5"/>
       <queryTableField id="6" name="Description" tableColumnId="6"/>
       <queryTableField id="9" name="DIGIKEY" tableColumnId="9"/>
+      <queryTableField id="29" dataBound="0" tableColumnId="7"/>
       <queryTableField id="28" name="Column1" tableColumnId="28"/>
     </queryTableFields>
     <queryTableDeletedFields count="20">
@@ -1805,20 +1853,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="BOM_watchplb_mainboard_v1_03" displayName="BOM_watchplb_mainboard_v1_03" ref="A1:H94" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H94" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState ref="A2:H92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="BOM_watchplb_mainboard_v1_03" displayName="BOM_watchplb_mainboard_v1_03" ref="A1:I94" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I94" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState ref="A2:I92">
     <sortCondition ref="E1:E92"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Qty" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="DIGIKEY" queryTableFieldId="9" dataDxfId="7"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" uniqueName="28" name="Link" queryTableFieldId="28" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="DIGIKEY" queryTableFieldId="9" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{DF968755-262E-4F9D-9ADD-8DBD0115DAD9}" uniqueName="7" name="Vorhanden" queryTableFieldId="29" dataDxfId="3"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" uniqueName="28" name="Link" queryTableFieldId="28" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1829,12 +1878,12 @@
   <autoFilter ref="A1:G7" xr:uid="{7D68FBC4-7B3B-4090-B9EB-BEEDFF2017AE}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{30D76A32-5A99-4726-87D1-A7B54F6F5170}" uniqueName="1" name="Qty" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{CC80E25E-2EBA-4559-A2DC-78E6B486A7F2}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{64AA79BA-24B6-4244-9D09-C929527D0F36}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B47DDA06-F190-4C2B-B33B-E48679806242}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{EF60C91C-5A23-4396-A103-0FB7FC4449C3}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{9DF9944F-766E-4088-A229-AD8E879A64B8}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B33B0B0F-1682-4D7A-A28E-C0261829F10E}" uniqueName="7" name="Bezugsquelle" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{CC80E25E-2EBA-4559-A2DC-78E6B486A7F2}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{64AA79BA-24B6-4244-9D09-C929527D0F36}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{B47DDA06-F190-4C2B-B33B-E48679806242}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{EF60C91C-5A23-4396-A103-0FB7FC4449C3}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{9DF9944F-766E-4088-A229-AD8E879A64B8}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{B33B0B0F-1682-4D7A-A28E-C0261829F10E}" uniqueName="7" name="Bezugsquelle" queryTableFieldId="9" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2137,10 +2186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,11 +2199,12 @@
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="177.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2177,10 +2227,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>22</v>
       </c>
@@ -2202,11 +2255,12 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -2228,11 +2282,14 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2254,11 +2311,12 @@
       <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2280,11 +2338,14 @@
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2306,11 +2367,14 @@
       <c r="G6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2332,11 +2396,14 @@
       <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2358,11 +2425,14 @@
       <c r="G8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2384,11 +2454,14 @@
       <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2410,11 +2483,14 @@
       <c r="G10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2436,11 +2512,14 @@
       <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2462,11 +2541,14 @@
       <c r="G12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2488,11 +2570,12 @@
       <c r="G13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2514,11 +2597,14 @@
       <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -2540,11 +2626,14 @@
       <c r="G15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2566,11 +2655,14 @@
       <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2592,11 +2684,14 @@
       <c r="G17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2618,11 +2713,14 @@
       <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2644,11 +2742,14 @@
       <c r="G19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2670,11 +2771,12 @@
       <c r="G20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2696,11 +2798,14 @@
       <c r="G21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2722,11 +2827,14 @@
       <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2748,11 +2856,14 @@
       <c r="G23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2774,11 +2885,14 @@
       <c r="G24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -2800,11 +2914,14 @@
       <c r="G25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2826,11 +2943,14 @@
       <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2852,11 +2972,14 @@
       <c r="G27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2878,11 +3001,14 @@
       <c r="G28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2904,11 +3030,12 @@
       <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2930,11 +3057,14 @@
       <c r="G30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2956,11 +3086,14 @@
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2982,11 +3115,14 @@
       <c r="G32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -3008,11 +3144,14 @@
       <c r="G33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3034,11 +3173,14 @@
       <c r="G34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3060,11 +3202,14 @@
       <c r="G35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -3086,11 +3231,14 @@
       <c r="G36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3112,11 +3260,14 @@
       <c r="G37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -3138,11 +3289,14 @@
       <c r="G38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3164,11 +3318,12 @@
       <c r="G39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -3190,11 +3345,14 @@
       <c r="G40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -3216,11 +3374,14 @@
       <c r="G41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I41" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -3242,11 +3403,14 @@
       <c r="G42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I42" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3268,11 +3432,14 @@
       <c r="G43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H43" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3294,11 +3461,14 @@
       <c r="G44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I44" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -3320,11 +3490,14 @@
       <c r="G45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I45" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3346,11 +3519,14 @@
       <c r="G46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I46" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5</v>
       </c>
@@ -3372,11 +3548,14 @@
       <c r="G47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="H47" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3398,11 +3577,14 @@
       <c r="G48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I48" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -3424,11 +3606,14 @@
       <c r="G49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3450,11 +3635,12 @@
       <c r="G50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -3476,11 +3662,14 @@
       <c r="G51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -3502,11 +3691,14 @@
       <c r="G52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="H52" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3528,11 +3720,14 @@
       <c r="G53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="H53" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3554,11 +3749,14 @@
       <c r="G54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H54" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -3580,11 +3778,14 @@
       <c r="G55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="H55" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9</v>
       </c>
@@ -3606,11 +3807,14 @@
       <c r="G56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I56" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -3632,11 +3836,14 @@
       <c r="G57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I57" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -3658,11 +3865,14 @@
       <c r="G58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="H58" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -3682,11 +3892,14 @@
         <v>31</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="2" t="s">
+      <c r="H59" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I59" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -3708,11 +3921,14 @@
       <c r="G60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="H60" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I60" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5</v>
       </c>
@@ -3734,11 +3950,14 @@
       <c r="G61" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="H61" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -3760,11 +3979,14 @@
       <c r="G62" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -3786,11 +4008,14 @@
       <c r="G63" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="H63" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I63" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1</v>
       </c>
@@ -3812,11 +4037,14 @@
       <c r="G64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="H64" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5</v>
       </c>
@@ -3838,11 +4066,14 @@
       <c r="G65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="H65" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I65" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5</v>
       </c>
@@ -3864,11 +4095,14 @@
       <c r="G66" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I66" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1</v>
       </c>
@@ -3890,11 +4124,14 @@
       <c r="G67" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="H67" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I67" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -3916,11 +4153,14 @@
       <c r="G68" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
       </c>
@@ -3942,11 +4182,14 @@
       <c r="G69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="H69" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I69" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1</v>
       </c>
@@ -3968,11 +4211,14 @@
       <c r="G70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H70" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I70" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1</v>
       </c>
@@ -3994,11 +4240,14 @@
       <c r="G71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="H71" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I71" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1</v>
       </c>
@@ -4020,11 +4269,14 @@
       <c r="G72" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="H72" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>14</v>
       </c>
@@ -4046,11 +4298,14 @@
       <c r="G73" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="H73" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I73" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1</v>
       </c>
@@ -4072,11 +4327,14 @@
       <c r="G74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -4098,11 +4356,14 @@
       <c r="G75" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I75" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1</v>
       </c>
@@ -4124,11 +4385,14 @@
       <c r="G76" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="H76" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I76" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1</v>
       </c>
@@ -4150,11 +4414,14 @@
       <c r="G77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="H77" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I77" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3</v>
       </c>
@@ -4176,11 +4443,14 @@
       <c r="G78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1</v>
       </c>
@@ -4202,11 +4472,12 @@
       <c r="G79" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="H79" s="1"/>
+      <c r="I79" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5</v>
       </c>
@@ -4228,11 +4499,14 @@
       <c r="G80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H80" s="2" t="s">
+      <c r="H80" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I80" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1</v>
       </c>
@@ -4254,11 +4528,14 @@
       <c r="G81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="H81" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I81" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1</v>
       </c>
@@ -4280,11 +4557,14 @@
       <c r="G82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H82" s="2" t="s">
+      <c r="H82" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I82" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1</v>
       </c>
@@ -4306,11 +4586,14 @@
       <c r="G83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="H83" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I83" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1</v>
       </c>
@@ -4332,11 +4615,14 @@
       <c r="G84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="H84" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="I84" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1</v>
       </c>
@@ -4358,11 +4644,14 @@
       <c r="G85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="H85" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1</v>
       </c>
@@ -4384,11 +4673,14 @@
       <c r="G86" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="H86" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -4396,8 +4688,9 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1</v>
       </c>
@@ -4409,11 +4702,14 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
-      <c r="H88" s="2" t="s">
+      <c r="H88" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I88" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4</v>
       </c>
@@ -4425,11 +4721,14 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
-      <c r="H89" s="2" t="s">
+      <c r="H89" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I89" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1</v>
       </c>
@@ -4441,11 +4740,14 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
-      <c r="H90" s="2" t="s">
+      <c r="H90" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I90" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1</v>
       </c>
@@ -4459,11 +4761,14 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
-      <c r="H91" s="2" t="s">
+      <c r="H91" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I91" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>3</v>
       </c>
@@ -4475,11 +4780,14 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
-      <c r="H92" s="3" t="s">
+      <c r="H92" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="I92" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -4491,11 +4799,14 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
-      <c r="H93" s="2" t="s">
+      <c r="H93" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I93" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1</v>
       </c>
@@ -4507,96 +4818,107 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
-      <c r="H94" s="2" t="s">
+      <c r="H94" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I94" s="2" t="s">
         <v>365</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:H94">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"n"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{AF0345A8-B47C-4869-919B-269F6D651AE3}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{C731202E-8C42-4533-9430-D0D210D2F04D}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{F4B8B8C2-7B71-442E-BD30-E2ECDE52B83C}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{D14FB558-0400-4498-92C4-56B46D21BC22}"/>
-    <hyperlink ref="H8" r:id="rId5" xr:uid="{5DD362B4-5F1C-4FDC-A987-A82743A44EA8}"/>
-    <hyperlink ref="H9" r:id="rId6" xr:uid="{9CEAE529-3EC7-4F41-93A5-282F18841EDE}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{F48F8CFD-B0D9-4AFE-B152-21E16506E0A7}"/>
-    <hyperlink ref="H11" r:id="rId8" xr:uid="{353243A0-006C-46E4-BD7C-B30694C373BD}"/>
-    <hyperlink ref="H12" r:id="rId9" xr:uid="{270A1B97-0628-47B6-8247-FCF5ED57D4EA}"/>
-    <hyperlink ref="H14" r:id="rId10" xr:uid="{430DC2A1-1AF3-464C-85EA-205ABD0234E1}"/>
-    <hyperlink ref="H15" r:id="rId11" xr:uid="{EA9CF757-3C5D-4A9E-9722-C1324684617C}"/>
-    <hyperlink ref="H16" r:id="rId12" xr:uid="{EC1FED56-AE0A-4603-B111-652B5FEC2199}"/>
-    <hyperlink ref="H17" r:id="rId13" xr:uid="{52F16938-ABED-435B-9CCA-6138A9D618D9}"/>
-    <hyperlink ref="H18" r:id="rId14" xr:uid="{47E845A0-F387-40D7-96A9-B9478EE14C94}"/>
-    <hyperlink ref="H19" r:id="rId15" xr:uid="{B20D9231-75FB-4C43-8059-163789FF26F6}"/>
-    <hyperlink ref="H21" r:id="rId16" xr:uid="{E13EAB3E-E0AC-4D49-89D9-0CF73C396A00}"/>
-    <hyperlink ref="H22" r:id="rId17" xr:uid="{2D3FE28D-C210-47AC-BC64-10C0F6F2BB42}"/>
-    <hyperlink ref="H23" r:id="rId18" xr:uid="{1C970058-6948-43F5-A099-2DB6A8AC01D4}"/>
-    <hyperlink ref="H24" r:id="rId19" xr:uid="{7C2AFDF6-564A-4EA2-906A-CCE9089BEA72}"/>
-    <hyperlink ref="H25" r:id="rId20" xr:uid="{2AEFDF37-2563-4BCA-9D9E-1445C812818E}"/>
-    <hyperlink ref="H27" r:id="rId21" xr:uid="{0C3AB61F-F931-4786-8A8A-1EB693DA3CFF}"/>
-    <hyperlink ref="H26" r:id="rId22" xr:uid="{1477C2DA-3FE5-4660-82D8-518113563D93}"/>
-    <hyperlink ref="H28" r:id="rId23" xr:uid="{C4B1E981-34A6-4EF7-B00C-15C58A7B4987}"/>
-    <hyperlink ref="H30" r:id="rId24" xr:uid="{ADCDF6A2-5C29-4188-A1C0-5F3CF20DB6FC}"/>
-    <hyperlink ref="H31" r:id="rId25" xr:uid="{E81595DD-8816-47A0-964D-2312E5F45F52}"/>
-    <hyperlink ref="H32" r:id="rId26" xr:uid="{9EB4D674-C238-432D-9ED4-8F0F1FE664D3}"/>
-    <hyperlink ref="H33" r:id="rId27" xr:uid="{FCB9527C-3E20-4150-8E3C-3FC277FC6717}"/>
-    <hyperlink ref="H34" r:id="rId28" xr:uid="{A312DCD4-F05C-4094-B9DD-B252B256BE76}"/>
-    <hyperlink ref="H35" r:id="rId29" xr:uid="{638C1B80-FD8C-4F30-BB95-86A2ED7D0422}"/>
-    <hyperlink ref="H36" r:id="rId30" xr:uid="{ED7FA15F-C5D1-4CE6-A2A5-F0C3249285DF}"/>
-    <hyperlink ref="H37" r:id="rId31" xr:uid="{2402B262-DED5-47FE-A686-F1BA8C2B2BB5}"/>
-    <hyperlink ref="H38" r:id="rId32" xr:uid="{586913CF-9E67-4EA9-86A5-94F9D2FC0DAA}"/>
-    <hyperlink ref="H40" r:id="rId33" xr:uid="{99FF5EC5-2D07-4E0C-91DC-4E5C10D67088}"/>
-    <hyperlink ref="H41" r:id="rId34" xr:uid="{63C0D3D9-7DDC-4EFE-97FD-A4807C0E6F6A}"/>
-    <hyperlink ref="H42" r:id="rId35" xr:uid="{3E9B107F-4128-40A2-A7DB-B6F6514EC076}"/>
-    <hyperlink ref="H43" r:id="rId36" xr:uid="{70FDA59E-BB39-4814-B256-4989EFD4D65B}"/>
-    <hyperlink ref="H44" r:id="rId37" xr:uid="{FD84E09B-1954-4181-8210-C7289913CA4B}"/>
-    <hyperlink ref="H45" r:id="rId38" xr:uid="{05BE3011-B7B8-461D-91DF-33A95EF67B21}"/>
-    <hyperlink ref="H46" r:id="rId39" xr:uid="{DF528EB6-EFE2-4D96-9170-41120432D00E}"/>
-    <hyperlink ref="H47" r:id="rId40" xr:uid="{6F870EFA-D99F-45E0-B630-693950A75E6A}"/>
-    <hyperlink ref="H48" r:id="rId41" xr:uid="{6B1A1121-0B1A-494D-BCF6-F1D8BB0BCD67}"/>
-    <hyperlink ref="H49" r:id="rId42" xr:uid="{95021D73-ED2D-46D7-8F5A-709B32274CD9}"/>
-    <hyperlink ref="H51" r:id="rId43" xr:uid="{EDC256D1-54B7-4C44-A294-829D6F1BFFC7}"/>
-    <hyperlink ref="H52" r:id="rId44" xr:uid="{D041C63D-6CF1-4142-B15A-330A8A6F3CDE}"/>
-    <hyperlink ref="H53" r:id="rId45" xr:uid="{33A140F6-DAFD-4D25-A9AE-D75B92F43B28}"/>
-    <hyperlink ref="H54" r:id="rId46" xr:uid="{EA5799EB-19FC-4564-A18B-D282479B64CB}"/>
-    <hyperlink ref="H55" r:id="rId47" xr:uid="{9EA1E006-7DA7-4472-955F-0F5C33D3EB6B}"/>
-    <hyperlink ref="H56" r:id="rId48" xr:uid="{22B28C6E-B7E8-41F8-95DD-1C286685B240}"/>
-    <hyperlink ref="H57" r:id="rId49" xr:uid="{69928788-C38D-4E2F-BBE3-3D75CD1C7F26}"/>
-    <hyperlink ref="H58" r:id="rId50" xr:uid="{D3636742-8C49-4ACB-BB67-52FE9655B217}"/>
-    <hyperlink ref="H59" r:id="rId51" xr:uid="{97111B7B-DD10-4B99-86B9-0BE4EDBFCD8F}"/>
-    <hyperlink ref="H60" r:id="rId52" xr:uid="{20159129-A44B-4E97-BA02-AD1FBFEA4B69}"/>
-    <hyperlink ref="H61" r:id="rId53" xr:uid="{3CED28F1-AABF-416E-B7C0-ECC43DCDAC62}"/>
-    <hyperlink ref="H62" r:id="rId54" xr:uid="{C81370BE-0069-4261-BE3D-BF8B150DEE89}"/>
-    <hyperlink ref="H63" r:id="rId55" xr:uid="{E0B7343B-5026-490A-9204-466DBBB9ADAE}"/>
-    <hyperlink ref="H64" r:id="rId56" xr:uid="{05D5C180-3052-47BC-AABA-0DD8BFCB4873}"/>
-    <hyperlink ref="H65" r:id="rId57" xr:uid="{ECD229B1-03EB-40FB-BBA9-E666914BCCAB}"/>
-    <hyperlink ref="H66" r:id="rId58" xr:uid="{AD71A0A8-3115-4953-A87D-C5D48968888C}"/>
-    <hyperlink ref="H67" r:id="rId59" xr:uid="{622363FB-A60E-446E-8FCE-8DDCE19A404F}"/>
-    <hyperlink ref="H68" r:id="rId60" xr:uid="{6DA95BE5-4C22-4731-AC62-C03F378988C7}"/>
-    <hyperlink ref="H69" r:id="rId61" xr:uid="{9B309B5B-516E-4DA9-B4B8-FF1CD77D3844}"/>
-    <hyperlink ref="H70" r:id="rId62" xr:uid="{AA20CDF6-47E2-4EF2-9EE2-0201B5D172ED}"/>
-    <hyperlink ref="H71" r:id="rId63" xr:uid="{73D88107-2063-4D16-836A-D7DD35FA8BA8}"/>
-    <hyperlink ref="H72" r:id="rId64" xr:uid="{9E318F0C-E499-4B2B-85ED-3963EE54841E}"/>
-    <hyperlink ref="H73" r:id="rId65" xr:uid="{909861B1-D635-41F1-BD4E-40B058473D5A}"/>
-    <hyperlink ref="H74" r:id="rId66" xr:uid="{465EFED6-9A1B-4BD9-952F-75D09E5D25EE}"/>
-    <hyperlink ref="H75" r:id="rId67" xr:uid="{416C2F72-C77B-4EE8-B622-F8E724523A30}"/>
-    <hyperlink ref="H76" r:id="rId68" xr:uid="{85DE1729-6FAF-4820-AE38-320843B10186}"/>
-    <hyperlink ref="H77" r:id="rId69" xr:uid="{7C46EF45-5CD2-4A6E-945D-DE761A89A429}"/>
-    <hyperlink ref="H78" r:id="rId70" xr:uid="{02BBC9EC-E9DD-41C4-BC24-B2986AD5B9ED}"/>
-    <hyperlink ref="H80" r:id="rId71" xr:uid="{51FD0953-0962-44B3-86A6-C0E840701570}"/>
-    <hyperlink ref="H81" r:id="rId72" xr:uid="{A7F0B3B6-A3DA-454D-9748-93D7C4294B16}"/>
-    <hyperlink ref="H82" r:id="rId73" xr:uid="{2E3D0B77-7944-4A58-BD92-7FDEFC567861}"/>
-    <hyperlink ref="H83" r:id="rId74" xr:uid="{23261957-D858-4C70-BE6B-45CF4C6D6A04}"/>
-    <hyperlink ref="H84" r:id="rId75" xr:uid="{5F90D62B-78D4-4DC4-B38B-033AFCA1A8A9}"/>
-    <hyperlink ref="H85" r:id="rId76" xr:uid="{A504FDA2-C5C6-437E-835B-C43549C397A5}"/>
-    <hyperlink ref="H86" r:id="rId77" xr:uid="{E30E8BEE-4700-4B4A-ADB5-2B9D5B123727}"/>
-    <hyperlink ref="H88" r:id="rId78" xr:uid="{B4C04F62-26E8-4A7F-8AF1-4502D45146C8}"/>
-    <hyperlink ref="H89" r:id="rId79" xr:uid="{981D863F-2D25-43CE-92B9-6104289E0E6C}"/>
-    <hyperlink ref="H90" r:id="rId80" xr:uid="{382606B6-F67A-47CA-B140-40CE51AA82AC}"/>
-    <hyperlink ref="H91" r:id="rId81" xr:uid="{A9695FEE-1C75-4F90-B13E-9F4D6A52FD46}"/>
-    <hyperlink ref="H92" r:id="rId82" xr:uid="{BCFCA6A7-8CB0-4BF2-B401-615C1F791D76}"/>
-    <hyperlink ref="H93" r:id="rId83" xr:uid="{8E2F0C3D-26F9-46EE-87C0-128291A42BE6}"/>
-    <hyperlink ref="H94" r:id="rId84" xr:uid="{49DAD614-9220-4A57-B6FD-961940DBADD0}"/>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{AF0345A8-B47C-4869-919B-269F6D651AE3}"/>
+    <hyperlink ref="I5" r:id="rId2" xr:uid="{C731202E-8C42-4533-9430-D0D210D2F04D}"/>
+    <hyperlink ref="I6" r:id="rId3" xr:uid="{F4B8B8C2-7B71-442E-BD30-E2ECDE52B83C}"/>
+    <hyperlink ref="I7" r:id="rId4" xr:uid="{D14FB558-0400-4498-92C4-56B46D21BC22}"/>
+    <hyperlink ref="I8" r:id="rId5" xr:uid="{5DD362B4-5F1C-4FDC-A987-A82743A44EA8}"/>
+    <hyperlink ref="I9" r:id="rId6" xr:uid="{9CEAE529-3EC7-4F41-93A5-282F18841EDE}"/>
+    <hyperlink ref="I10" r:id="rId7" xr:uid="{F48F8CFD-B0D9-4AFE-B152-21E16506E0A7}"/>
+    <hyperlink ref="I11" r:id="rId8" xr:uid="{353243A0-006C-46E4-BD7C-B30694C373BD}"/>
+    <hyperlink ref="I12" r:id="rId9" xr:uid="{270A1B97-0628-47B6-8247-FCF5ED57D4EA}"/>
+    <hyperlink ref="I14" r:id="rId10" xr:uid="{430DC2A1-1AF3-464C-85EA-205ABD0234E1}"/>
+    <hyperlink ref="I15" r:id="rId11" xr:uid="{EA9CF757-3C5D-4A9E-9722-C1324684617C}"/>
+    <hyperlink ref="I16" r:id="rId12" xr:uid="{EC1FED56-AE0A-4603-B111-652B5FEC2199}"/>
+    <hyperlink ref="I17" r:id="rId13" xr:uid="{52F16938-ABED-435B-9CCA-6138A9D618D9}"/>
+    <hyperlink ref="I18" r:id="rId14" xr:uid="{47E845A0-F387-40D7-96A9-B9478EE14C94}"/>
+    <hyperlink ref="I19" r:id="rId15" xr:uid="{B20D9231-75FB-4C43-8059-163789FF26F6}"/>
+    <hyperlink ref="I21" r:id="rId16" xr:uid="{E13EAB3E-E0AC-4D49-89D9-0CF73C396A00}"/>
+    <hyperlink ref="I22" r:id="rId17" xr:uid="{2D3FE28D-C210-47AC-BC64-10C0F6F2BB42}"/>
+    <hyperlink ref="I23" r:id="rId18" xr:uid="{1C970058-6948-43F5-A099-2DB6A8AC01D4}"/>
+    <hyperlink ref="I24" r:id="rId19" xr:uid="{7C2AFDF6-564A-4EA2-906A-CCE9089BEA72}"/>
+    <hyperlink ref="I25" r:id="rId20" xr:uid="{2AEFDF37-2563-4BCA-9D9E-1445C812818E}"/>
+    <hyperlink ref="I27" r:id="rId21" xr:uid="{0C3AB61F-F931-4786-8A8A-1EB693DA3CFF}"/>
+    <hyperlink ref="I26" r:id="rId22" xr:uid="{1477C2DA-3FE5-4660-82D8-518113563D93}"/>
+    <hyperlink ref="I28" r:id="rId23" xr:uid="{C4B1E981-34A6-4EF7-B00C-15C58A7B4987}"/>
+    <hyperlink ref="I30" r:id="rId24" xr:uid="{ADCDF6A2-5C29-4188-A1C0-5F3CF20DB6FC}"/>
+    <hyperlink ref="I31" r:id="rId25" xr:uid="{E81595DD-8816-47A0-964D-2312E5F45F52}"/>
+    <hyperlink ref="I32" r:id="rId26" xr:uid="{9EB4D674-C238-432D-9ED4-8F0F1FE664D3}"/>
+    <hyperlink ref="I33" r:id="rId27" xr:uid="{FCB9527C-3E20-4150-8E3C-3FC277FC6717}"/>
+    <hyperlink ref="I34" r:id="rId28" xr:uid="{A312DCD4-F05C-4094-B9DD-B252B256BE76}"/>
+    <hyperlink ref="I35" r:id="rId29" xr:uid="{638C1B80-FD8C-4F30-BB95-86A2ED7D0422}"/>
+    <hyperlink ref="I36" r:id="rId30" xr:uid="{ED7FA15F-C5D1-4CE6-A2A5-F0C3249285DF}"/>
+    <hyperlink ref="I37" r:id="rId31" xr:uid="{2402B262-DED5-47FE-A686-F1BA8C2B2BB5}"/>
+    <hyperlink ref="I38" r:id="rId32" xr:uid="{586913CF-9E67-4EA9-86A5-94F9D2FC0DAA}"/>
+    <hyperlink ref="I40" r:id="rId33" xr:uid="{99FF5EC5-2D07-4E0C-91DC-4E5C10D67088}"/>
+    <hyperlink ref="I41" r:id="rId34" xr:uid="{63C0D3D9-7DDC-4EFE-97FD-A4807C0E6F6A}"/>
+    <hyperlink ref="I42" r:id="rId35" xr:uid="{3E9B107F-4128-40A2-A7DB-B6F6514EC076}"/>
+    <hyperlink ref="I43" r:id="rId36" xr:uid="{70FDA59E-BB39-4814-B256-4989EFD4D65B}"/>
+    <hyperlink ref="I44" r:id="rId37" xr:uid="{FD84E09B-1954-4181-8210-C7289913CA4B}"/>
+    <hyperlink ref="I45" r:id="rId38" xr:uid="{05BE3011-B7B8-461D-91DF-33A95EF67B21}"/>
+    <hyperlink ref="I46" r:id="rId39" xr:uid="{DF528EB6-EFE2-4D96-9170-41120432D00E}"/>
+    <hyperlink ref="I47" r:id="rId40" xr:uid="{6F870EFA-D99F-45E0-B630-693950A75E6A}"/>
+    <hyperlink ref="I48" r:id="rId41" xr:uid="{6B1A1121-0B1A-494D-BCF6-F1D8BB0BCD67}"/>
+    <hyperlink ref="I49" r:id="rId42" xr:uid="{95021D73-ED2D-46D7-8F5A-709B32274CD9}"/>
+    <hyperlink ref="I51" r:id="rId43" xr:uid="{EDC256D1-54B7-4C44-A294-829D6F1BFFC7}"/>
+    <hyperlink ref="I52" r:id="rId44" xr:uid="{D041C63D-6CF1-4142-B15A-330A8A6F3CDE}"/>
+    <hyperlink ref="I53" r:id="rId45" xr:uid="{33A140F6-DAFD-4D25-A9AE-D75B92F43B28}"/>
+    <hyperlink ref="I54" r:id="rId46" xr:uid="{EA5799EB-19FC-4564-A18B-D282479B64CB}"/>
+    <hyperlink ref="I55" r:id="rId47" xr:uid="{9EA1E006-7DA7-4472-955F-0F5C33D3EB6B}"/>
+    <hyperlink ref="I56" r:id="rId48" xr:uid="{22B28C6E-B7E8-41F8-95DD-1C286685B240}"/>
+    <hyperlink ref="I57" r:id="rId49" xr:uid="{69928788-C38D-4E2F-BBE3-3D75CD1C7F26}"/>
+    <hyperlink ref="I58" r:id="rId50" xr:uid="{D3636742-8C49-4ACB-BB67-52FE9655B217}"/>
+    <hyperlink ref="I59" r:id="rId51" xr:uid="{97111B7B-DD10-4B99-86B9-0BE4EDBFCD8F}"/>
+    <hyperlink ref="I60" r:id="rId52" xr:uid="{20159129-A44B-4E97-BA02-AD1FBFEA4B69}"/>
+    <hyperlink ref="I61" r:id="rId53" xr:uid="{3CED28F1-AABF-416E-B7C0-ECC43DCDAC62}"/>
+    <hyperlink ref="I62" r:id="rId54" xr:uid="{C81370BE-0069-4261-BE3D-BF8B150DEE89}"/>
+    <hyperlink ref="I63" r:id="rId55" xr:uid="{E0B7343B-5026-490A-9204-466DBBB9ADAE}"/>
+    <hyperlink ref="I64" r:id="rId56" xr:uid="{05D5C180-3052-47BC-AABA-0DD8BFCB4873}"/>
+    <hyperlink ref="I65" r:id="rId57" xr:uid="{ECD229B1-03EB-40FB-BBA9-E666914BCCAB}"/>
+    <hyperlink ref="I66" r:id="rId58" xr:uid="{AD71A0A8-3115-4953-A87D-C5D48968888C}"/>
+    <hyperlink ref="I67" r:id="rId59" xr:uid="{622363FB-A60E-446E-8FCE-8DDCE19A404F}"/>
+    <hyperlink ref="I68" r:id="rId60" xr:uid="{6DA95BE5-4C22-4731-AC62-C03F378988C7}"/>
+    <hyperlink ref="I69" r:id="rId61" xr:uid="{9B309B5B-516E-4DA9-B4B8-FF1CD77D3844}"/>
+    <hyperlink ref="I70" r:id="rId62" xr:uid="{AA20CDF6-47E2-4EF2-9EE2-0201B5D172ED}"/>
+    <hyperlink ref="I71" r:id="rId63" xr:uid="{73D88107-2063-4D16-836A-D7DD35FA8BA8}"/>
+    <hyperlink ref="I72" r:id="rId64" xr:uid="{9E318F0C-E499-4B2B-85ED-3963EE54841E}"/>
+    <hyperlink ref="I73" r:id="rId65" xr:uid="{909861B1-D635-41F1-BD4E-40B058473D5A}"/>
+    <hyperlink ref="I74" r:id="rId66" xr:uid="{465EFED6-9A1B-4BD9-952F-75D09E5D25EE}"/>
+    <hyperlink ref="I75" r:id="rId67" xr:uid="{416C2F72-C77B-4EE8-B622-F8E724523A30}"/>
+    <hyperlink ref="I76" r:id="rId68" xr:uid="{85DE1729-6FAF-4820-AE38-320843B10186}"/>
+    <hyperlink ref="I77" r:id="rId69" xr:uid="{7C46EF45-5CD2-4A6E-945D-DE761A89A429}"/>
+    <hyperlink ref="I78" r:id="rId70" xr:uid="{02BBC9EC-E9DD-41C4-BC24-B2986AD5B9ED}"/>
+    <hyperlink ref="I80" r:id="rId71" xr:uid="{51FD0953-0962-44B3-86A6-C0E840701570}"/>
+    <hyperlink ref="I81" r:id="rId72" xr:uid="{A7F0B3B6-A3DA-454D-9748-93D7C4294B16}"/>
+    <hyperlink ref="I82" r:id="rId73" xr:uid="{2E3D0B77-7944-4A58-BD92-7FDEFC567861}"/>
+    <hyperlink ref="I83" r:id="rId74" xr:uid="{23261957-D858-4C70-BE6B-45CF4C6D6A04}"/>
+    <hyperlink ref="I84" r:id="rId75" xr:uid="{5F90D62B-78D4-4DC4-B38B-033AFCA1A8A9}"/>
+    <hyperlink ref="I85" r:id="rId76" xr:uid="{A504FDA2-C5C6-437E-835B-C43549C397A5}"/>
+    <hyperlink ref="I86" r:id="rId77" xr:uid="{E30E8BEE-4700-4B4A-ADB5-2B9D5B123727}"/>
+    <hyperlink ref="I88" r:id="rId78" xr:uid="{B4C04F62-26E8-4A7F-8AF1-4502D45146C8}"/>
+    <hyperlink ref="I89" r:id="rId79" xr:uid="{981D863F-2D25-43CE-92B9-6104289E0E6C}"/>
+    <hyperlink ref="I90" r:id="rId80" xr:uid="{382606B6-F67A-47CA-B140-40CE51AA82AC}"/>
+    <hyperlink ref="I91" r:id="rId81" xr:uid="{A9695FEE-1C75-4F90-B13E-9F4D6A52FD46}"/>
+    <hyperlink ref="I92" r:id="rId82" xr:uid="{BCFCA6A7-8CB0-4BF2-B401-615C1F791D76}"/>
+    <hyperlink ref="I93" r:id="rId83" xr:uid="{8E2F0C3D-26F9-46EE-87C0-128291A42BE6}"/>
+    <hyperlink ref="I94" r:id="rId84" xr:uid="{49DAD614-9220-4A57-B6FD-961940DBADD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId85"/>

</xml_diff>